<commit_message>
tests version control of .xlsx files
</commit_message>
<xml_diff>
--- a/Scripts/WOI.xlsx
+++ b/Scripts/WOI.xlsx
@@ -346,10 +346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,6 +404,17 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1003</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.64304398148148145</v>
+      </c>
+      <c r="C5">
+        <v>0.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adds more test entries
</commit_message>
<xml_diff>
--- a/Scripts/WOI.xlsx
+++ b/Scripts/WOI.xlsx
@@ -346,10 +346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,6 +415,28 @@
         <v>0.25</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>121</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.46552083333333333</v>
+      </c>
+      <c r="C6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>121</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.46249999999999997</v>
+      </c>
+      <c r="C7">
+        <v>0.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add test entries from 2 folders, 4 different animals
</commit_message>
<xml_diff>
--- a/Scripts/WOI.xlsx
+++ b/Scripts/WOI.xlsx
@@ -346,10 +346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +437,74 @@
         <v>0.4</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>121</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.46574074074074073</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>163</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.46521990740740743</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>164</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.68958333333333333</v>
+      </c>
+      <c r="C10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>164</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="C11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1071</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.69515046296296301</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1071</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.69269675925925922</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixes indexing bug if window starts at beginning of trace
</commit_message>
<xml_diff>
--- a/Scripts/WOI.xlsx
+++ b/Scripts/WOI.xlsx
@@ -346,10 +346,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,6 +503,72 @@
         <v>11</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>169</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.45688657407407413</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>169</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.45868055555555554</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>178</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.45682870370370371</v>
+      </c>
+      <c r="C16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>178</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.45682870370370371</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>178</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.45682870370370371</v>
+      </c>
+      <c r="C18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>178</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.45682870370370371</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
adds genotype number to the experiment-wide data structure
</commit_message>
<xml_diff>
--- a/Scripts/WOI.xlsx
+++ b/Scripts/WOI.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Animal ID</t>
   </si>
@@ -28,6 +28,12 @@
   </si>
   <si>
     <t>Length (min)</t>
+  </si>
+  <si>
+    <t>Genotype</t>
+  </si>
+  <si>
+    <t>Window #</t>
   </si>
 </sst>
 </file>
@@ -346,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -357,10 +363,11 @@
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -370,8 +377,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1002</v>
       </c>
@@ -381,8 +394,14 @@
       <c r="C2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -392,8 +411,14 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1002</v>
       </c>
@@ -403,8 +428,14 @@
       <c r="C4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1003</v>
       </c>
@@ -414,8 +445,14 @@
       <c r="C5">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>121</v>
       </c>
@@ -425,8 +462,14 @@
       <c r="C6">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>121</v>
       </c>
@@ -436,8 +479,14 @@
       <c r="C7">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>121</v>
       </c>
@@ -447,8 +496,14 @@
       <c r="C8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>163</v>
       </c>
@@ -458,8 +513,14 @@
       <c r="C9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>164</v>
       </c>
@@ -469,8 +530,14 @@
       <c r="C10">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>164</v>
       </c>
@@ -480,8 +547,14 @@
       <c r="C11">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1071</v>
       </c>
@@ -491,8 +564,14 @@
       <c r="C12">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1071</v>
       </c>
@@ -502,8 +581,14 @@
       <c r="C13">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>169</v>
       </c>
@@ -513,8 +598,14 @@
       <c r="C14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>169</v>
       </c>
@@ -524,8 +615,14 @@
       <c r="C15">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>178</v>
       </c>
@@ -535,8 +632,14 @@
       <c r="C16">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>178</v>
       </c>
@@ -546,8 +649,14 @@
       <c r="C17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>178</v>
       </c>
@@ -557,8 +666,14 @@
       <c r="C18">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>178</v>
       </c>
@@ -567,6 +682,12 @@
       </c>
       <c r="C19">
         <v>16</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
switches entry column order in WOI.xlsx
</commit_message>
<xml_diff>
--- a/Scripts/WOI.xlsx
+++ b/Scripts/WOI.xlsx
@@ -355,7 +355,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -372,322 +372,322 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1002</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
         <v>0.64223379629629629</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>0.5</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1002</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
         <v>0.64210648148148153</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1002</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
         <v>0.64234953703703701</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>0.5</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1003</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
         <v>0.64304398148148145</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>0.25</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>121</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
         <v>0.46552083333333333</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>0.25</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>121</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
         <v>0.46249999999999997</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>0.4</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>121</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
         <v>0.46574074074074073</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>7</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>163</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
         <v>0.46521990740740743</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>10</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>164</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
         <v>0.68958333333333333</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>11</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>164</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
         <v>0.69097222222222221</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>12</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1071</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
         <v>0.69515046296296301</v>
       </c>
-      <c r="C12">
+      <c r="E12">
         <v>6</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1071</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
         <v>0.69269675925925922</v>
       </c>
-      <c r="C13">
+      <c r="E13">
         <v>11</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>169</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
         <v>0.45688657407407413</v>
       </c>
-      <c r="C14">
+      <c r="E14">
         <v>13</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>169</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
         <v>0.45868055555555554</v>
       </c>
-      <c r="C15">
+      <c r="E15">
         <v>9</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>178</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
         <v>0.45682870370370371</v>
       </c>
-      <c r="C16">
+      <c r="E16">
         <v>22</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>178</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1">
         <v>0.45682870370370371</v>
       </c>
-      <c r="C17">
+      <c r="E17">
         <v>5</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>178</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
         <v>0.45682870370370371</v>
       </c>
-      <c r="C18">
+      <c r="E18">
         <v>14</v>
-      </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-      <c r="E18">
-        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>178</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
         <v>0.45682870370370371</v>
       </c>
-      <c r="C19">
+      <c r="E19">
         <v>16</v>
-      </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes scripts to label windows as specified in WOI.xlsx
</commit_message>
<xml_diff>
--- a/Scripts/WOI.xlsx
+++ b/Scripts/WOI.xlsx
@@ -352,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,10 +463,10 @@
         <v>2</v>
       </c>
       <c r="D6" s="1">
-        <v>0.46552083333333333</v>
+        <v>0.45925925925925926</v>
       </c>
       <c r="E6">
-        <v>0.25</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -483,7 +483,7 @@
         <v>0.46249999999999997</v>
       </c>
       <c r="E7">
-        <v>0.4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -500,7 +500,7 @@
         <v>0.46574074074074073</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -514,146 +514,146 @@
         <v>2</v>
       </c>
       <c r="D9" s="1">
-        <v>0.46521990740740743</v>
+        <v>0.45925925925925926</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1">
-        <v>0.68958333333333333</v>
+        <v>0.46249999999999997</v>
       </c>
       <c r="E10">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1">
-        <v>0.69097222222222221</v>
+        <v>0.46574074074074073</v>
       </c>
       <c r="E11">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1071</v>
+        <v>164</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1">
-        <v>0.69515046296296301</v>
+        <v>0.68958333333333333</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1071</v>
+        <v>164</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1">
-        <v>0.69269675925925922</v>
+        <v>0.69097222222222221</v>
       </c>
       <c r="E13">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>169</v>
+        <v>1071</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1">
-        <v>0.45688657407407413</v>
+        <v>0.69515046296296301</v>
       </c>
       <c r="E14">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>169</v>
+        <v>1071</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
-        <v>0.45868055555555554</v>
+        <v>0.69269675925925922</v>
       </c>
       <c r="E15">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1">
-        <v>0.45682870370370371</v>
+        <v>0.45688657407407413</v>
       </c>
       <c r="E16">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1">
-        <v>0.45682870370370371</v>
+        <v>0.45868055555555554</v>
       </c>
       <c r="E17">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>178</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -670,7 +670,7 @@
         <v>0.45682870370370371</v>
       </c>
       <c r="E18">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>178</v>
       </c>
       <c r="B19">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -687,6 +687,40 @@
         <v>0.45682870370370371</v>
       </c>
       <c r="E19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>178</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.45682870370370371</v>
+      </c>
+      <c r="E20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>178</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.45682870370370371</v>
+      </c>
+      <c r="E21">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
retrieves and uses values stored in windowDefinition
</commit_message>
<xml_diff>
--- a/Scripts/WOI.xlsx
+++ b/Scripts/WOI.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBDA2F6-9724-430B-84DD-EDC1DBA94726}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
reverts to absolute time specification for windowing, removes unneeded columns in .xlsx files
</commit_message>
<xml_diff>
--- a/Scripts/WOI.xlsx
+++ b/Scripts/WOI.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBBDA2F6-9724-430B-84DD-EDC1DBA94726}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E333200-88BD-4C4D-BA68-B65AC7366D3E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Animal ID</t>
   </si>
   <si>
     <t>Start Time</t>
-  </si>
-  <si>
-    <t>Length (min)</t>
   </si>
   <si>
     <t>Genotype</t>
@@ -353,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -368,24 +365,21 @@
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1002</v>
       </c>
@@ -398,11 +392,8 @@
       <c r="D2" s="1">
         <v>0.64223379629629629</v>
       </c>
-      <c r="E2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -415,11 +406,8 @@
       <c r="D3" s="1">
         <v>0.64210648148148153</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1002</v>
       </c>
@@ -432,11 +420,8 @@
       <c r="D4" s="1">
         <v>0.64234953703703701</v>
       </c>
-      <c r="E4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1003</v>
       </c>
@@ -449,11 +434,8 @@
       <c r="D5" s="1">
         <v>0.64304398148148145</v>
       </c>
-      <c r="E5">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>121</v>
       </c>
@@ -466,11 +448,8 @@
       <c r="D6" s="1">
         <v>0.45925925925925926</v>
       </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>121</v>
       </c>
@@ -483,11 +462,8 @@
       <c r="D7" s="1">
         <v>0.46249999999999997</v>
       </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>121</v>
       </c>
@@ -500,11 +476,8 @@
       <c r="D8" s="1">
         <v>0.46574074074074073</v>
       </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>163</v>
       </c>
@@ -517,11 +490,8 @@
       <c r="D9" s="1">
         <v>0.45925925925925926</v>
       </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>163</v>
       </c>
@@ -534,11 +504,8 @@
       <c r="D10" s="1">
         <v>0.46249999999999997</v>
       </c>
-      <c r="E10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>163</v>
       </c>
@@ -551,11 +518,8 @@
       <c r="D11" s="1">
         <v>0.46574074074074073</v>
       </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>164</v>
       </c>
@@ -568,11 +532,8 @@
       <c r="D12" s="1">
         <v>0.68958333333333333</v>
       </c>
-      <c r="E12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>164</v>
       </c>
@@ -585,11 +546,8 @@
       <c r="D13" s="1">
         <v>0.69097222222222221</v>
       </c>
-      <c r="E13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1071</v>
       </c>
@@ -602,11 +560,8 @@
       <c r="D14" s="1">
         <v>0.69515046296296301</v>
       </c>
-      <c r="E14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1071</v>
       </c>
@@ -619,11 +574,8 @@
       <c r="D15" s="1">
         <v>0.69269675925925922</v>
       </c>
-      <c r="E15">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>169</v>
       </c>
@@ -636,11 +588,8 @@
       <c r="D16" s="1">
         <v>0.45688657407407413</v>
       </c>
-      <c r="E16">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>169</v>
       </c>
@@ -653,11 +602,8 @@
       <c r="D17" s="1">
         <v>0.45868055555555554</v>
       </c>
-      <c r="E17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>178</v>
       </c>
@@ -670,11 +616,8 @@
       <c r="D18" s="1">
         <v>0.45682870370370371</v>
       </c>
-      <c r="E18">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>178</v>
       </c>
@@ -687,11 +630,8 @@
       <c r="D19" s="1">
         <v>0.45682870370370371</v>
       </c>
-      <c r="E19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>178</v>
       </c>
@@ -704,11 +644,8 @@
       <c r="D20" s="1">
         <v>0.45682870370370371</v>
       </c>
-      <c r="E20">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>178</v>
       </c>
@@ -720,9 +657,6 @@
       </c>
       <c r="D21" s="1">
         <v>0.45682870370370371</v>
-      </c>
-      <c r="E21">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds windows for real datasets
</commit_message>
<xml_diff>
--- a/Scripts/WOI.xlsx
+++ b/Scripts/WOI.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E333200-88BD-4C4D-BA68-B65AC7366D3E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27245F8C-C59F-4013-A93F-C7F06667C332}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -350,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,6 +659,34 @@
         <v>0.45682870370370371</v>
       </c>
     </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>998</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.53865740740740742</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>991</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.53865740740740742</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
correct power band calculations
</commit_message>
<xml_diff>
--- a/Scripts/WOI.xlsx
+++ b/Scripts/WOI.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27245F8C-C59F-4013-A93F-C7F06667C332}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380534A8-06D6-448E-985F-C3263B7C5A75}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -350,10 +350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,13 +678,41 @@
         <v>991</v>
       </c>
       <c r="B23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" s="1">
         <v>0.53865740740740742</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1061</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.48321759259259256</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1064</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.48321759259259256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fixes in the window type lengths for some of the test data
</commit_message>
<xml_diff>
--- a/Scripts/WOI.xlsx
+++ b/Scripts/WOI.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380534A8-06D6-448E-985F-C3263B7C5A75}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B148D5BD-DE19-47F0-A7B8-D064518FB65E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -353,7 +353,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,7 +398,7 @@
         <v>1002</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -432,7 +432,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="1">
-        <v>0.64304398148148145</v>
+        <v>0.64178240740740744</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
prints status messages outside of the function
</commit_message>
<xml_diff>
--- a/Scripts/WOI.xlsx
+++ b/Scripts/WOI.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B148D5BD-DE19-47F0-A7B8-D064518FB65E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6296FEF5-F242-41B2-8878-677CAC2E8050}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <t>Genotype</t>
   </si>
   <si>
-    <t>Window #</t>
+    <t>Window Type</t>
   </si>
 </sst>
 </file>
@@ -353,13 +353,13 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" customWidth="1"/>

</xml_diff>